<commit_message>
add the topic of Prof Tsai
</commit_message>
<xml_diff>
--- a/Admin/2015-TH-XLP-流程及计分规则.xlsx
+++ b/Admin/2015-TH-XLP-流程及计分规则.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="400" windowWidth="24820" windowHeight="13460"/>
+    <workbookView xWindow="0" yWindow="405" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1562,10 +1562,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>嘉宾演讲（大数据）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>14:16-14:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1845,6 +1841,10 @@
       <t xml:space="preserve">
 截止日期为2015年1月29日7：00。延时上交者取消展示资格</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘉宾演讲（Evolution of Software Design）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2399,6 +2399,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2415,47 +2451,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2760,27 +2760,27 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="23" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.875" style="31" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="35" customWidth="1"/>
     <col min="8" max="8" width="19" style="35" customWidth="1"/>
-    <col min="9" max="9" width="58.6640625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="49.6640625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="3" customWidth="1"/>
-    <col min="12" max="13" width="16.33203125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="3"/>
+    <col min="9" max="9" width="58.625" style="36" customWidth="1"/>
+    <col min="10" max="10" width="49.625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="3" customWidth="1"/>
+    <col min="12" max="13" width="16.375" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1">
+    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="24.75" customHeight="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2830,14 +2830,14 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="114" customHeight="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="68"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
@@ -2856,14 +2856,14 @@
       <c r="I3" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="67" t="s">
         <v>125</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="68" customHeight="1">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>153</v>
       </c>
@@ -2877,16 +2877,16 @@
       <c r="G4" s="38"/>
       <c r="H4" s="39"/>
       <c r="I4" s="40"/>
-      <c r="J4" s="56"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="74" customHeight="1">
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="62"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="11" t="s">
         <v>117</v>
       </c>
@@ -2899,16 +2899,16 @@
       </c>
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
-      <c r="J5" s="56"/>
-    </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" ht="93" customHeight="1">
+      <c r="J5" s="68"/>
+    </row>
+    <row r="6" spans="1:12" s="5" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="62"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="11" t="s">
         <v>117</v>
       </c>
@@ -2923,16 +2923,16 @@
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="40"/>
-      <c r="J6" s="57"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="99" customHeight="1">
+      <c r="J6" s="69"/>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="64" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -2951,14 +2951,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="188" customHeight="1">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="188.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="11" t="s">
         <v>117</v>
       </c>
@@ -2977,14 +2977,14 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" ht="48" customHeight="1">
+    <row r="9" spans="1:12" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="62"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="11" t="s">
         <v>117</v>
       </c>
@@ -3003,14 +3003,14 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="64.5" customHeight="1">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="62"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="11" t="s">
         <v>117</v>
       </c>
@@ -3030,14 +3030,14 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1">
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="11" t="s">
         <v>117</v>
       </c>
@@ -3054,14 +3054,14 @@
       <c r="I11" s="40"/>
       <c r="J11" s="44"/>
     </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" ht="117" customHeight="1">
+    <row r="12" spans="1:12" s="5" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="64"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="11" t="s">
         <v>108</v>
       </c>
@@ -3082,14 +3082,14 @@
       </c>
       <c r="J12" s="44"/>
     </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" ht="183" customHeight="1">
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="64"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="11" t="s">
         <v>117</v>
       </c>
@@ -3110,14 +3110,14 @@
       </c>
       <c r="J13" s="46"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="81" customHeight="1">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="11" t="s">
         <v>117</v>
       </c>
@@ -3138,14 +3138,14 @@
       </c>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="52" customHeight="1">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="62"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="11" t="s">
         <v>117</v>
       </c>
@@ -3160,14 +3160,14 @@
       <c r="I15" s="40"/>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="88" customHeight="1">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="62"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="11" t="s">
         <v>117</v>
       </c>
@@ -3182,18 +3182,18 @@
       </c>
       <c r="H16" s="39"/>
       <c r="I16" s="40"/>
-      <c r="J16" s="58" t="s">
+      <c r="J16" s="70" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="105.75" customHeight="1">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="C17" s="64"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="11" t="s">
         <v>117</v>
       </c>
@@ -3212,16 +3212,16 @@
       <c r="I17" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="J17" s="59"/>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="182" customHeight="1">
+      <c r="J17" s="71"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="182.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="11" t="s">
         <v>117</v>
       </c>
@@ -3240,16 +3240,16 @@
       <c r="I18" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="J18" s="60"/>
-    </row>
-    <row r="19" spans="1:10" s="5" customFormat="1" ht="98" customHeight="1">
+      <c r="J18" s="72"/>
+    </row>
+    <row r="19" spans="1:10" s="5" customFormat="1" ht="98.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="64"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="11" t="s">
         <v>117</v>
       </c>
@@ -3270,14 +3270,14 @@
       </c>
       <c r="J19" s="41"/>
     </row>
-    <row r="20" spans="1:10" s="5" customFormat="1" ht="203" customHeight="1">
+    <row r="20" spans="1:10" s="5" customFormat="1" ht="203.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="64"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="11" t="s">
         <v>117</v>
       </c>
@@ -3300,12 +3300,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1">
+    <row r="21" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="11"/>
       <c r="E21" s="17"/>
       <c r="F21" s="29"/>
@@ -3314,14 +3314,14 @@
       <c r="I21" s="40"/>
       <c r="J21" s="41"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="147" customHeight="1">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="70"/>
+      <c r="C22" s="62"/>
       <c r="D22" s="11" t="s">
         <v>22</v>
       </c>
@@ -3342,14 +3342,14 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1">
+    <row r="23" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="64"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="11" t="s">
         <v>117</v>
       </c>
@@ -3370,14 +3370,14 @@
       </c>
       <c r="J23" s="41"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="121" customHeight="1">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="62"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="11" t="s">
         <v>117</v>
       </c>
@@ -3392,14 +3392,14 @@
       <c r="I24" s="40"/>
       <c r="J24" s="41"/>
     </row>
-    <row r="25" spans="1:10" s="5" customFormat="1" ht="268" customHeight="1">
+    <row r="25" spans="1:10" s="5" customFormat="1" ht="267.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="62"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="11" t="s">
         <v>117</v>
       </c>
@@ -3418,14 +3418,14 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="117" customHeight="1">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="62"/>
+      <c r="C26" s="56"/>
       <c r="D26" s="11" t="s">
         <v>117</v>
       </c>
@@ -3446,14 +3446,14 @@
       </c>
       <c r="J26" s="41"/>
     </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="94.5" customHeight="1">
+    <row r="27" spans="1:10" s="2" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="62"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="11" t="s">
         <v>117</v>
       </c>
@@ -3470,14 +3470,14 @@
       </c>
       <c r="J27" s="41"/>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" ht="116.25" customHeight="1">
+    <row r="28" spans="1:10" s="2" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="C28" s="62"/>
+      <c r="C28" s="56"/>
       <c r="D28" s="11" t="s">
         <v>117</v>
       </c>
@@ -3492,14 +3492,14 @@
       <c r="I28" s="40"/>
       <c r="J28" s="41"/>
     </row>
-    <row r="29" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
+    <row r="29" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="64"/>
+      <c r="C29" s="66"/>
       <c r="D29" s="11" t="s">
         <v>117</v>
       </c>
@@ -3520,19 +3520,19 @@
       </c>
       <c r="J29" s="41"/>
     </row>
-    <row r="30" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
+    <row r="30" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="C30" s="62"/>
+      <c r="B30" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="56"/>
       <c r="D30" s="11" t="s">
         <v>117</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="38" t="s">
@@ -3544,14 +3544,14 @@
       </c>
       <c r="J30" s="41"/>
     </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
+    <row r="31" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="56"/>
       <c r="D31" s="11" t="s">
         <v>117</v>
       </c>
@@ -3570,14 +3570,14 @@
       </c>
       <c r="J31" s="41"/>
     </row>
-    <row r="32" spans="1:10" s="7" customFormat="1" ht="175" customHeight="1">
+    <row r="32" spans="1:10" s="7" customFormat="1" ht="174.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="64"/>
+      <c r="C32" s="66"/>
       <c r="D32" s="11" t="s">
         <v>117</v>
       </c>
@@ -3592,18 +3592,18 @@
         <v>5</v>
       </c>
       <c r="I32" s="40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J32" s="41" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1">
+    <row r="33" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="66"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="16"/>
       <c r="E33" s="18"/>
       <c r="F33" s="30"/>
@@ -3741,14 +3741,14 @@
       <c r="EH33" s="9"/>
       <c r="EI33" s="9"/>
     </row>
-    <row r="34" spans="1:139" s="2" customFormat="1" ht="117" customHeight="1">
+    <row r="34" spans="1:139" s="2" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="62"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="11" t="s">
         <v>117</v>
       </c>
@@ -3767,14 +3767,14 @@
       </c>
       <c r="J34" s="41"/>
     </row>
-    <row r="35" spans="1:139" s="2" customFormat="1" ht="64.5" customHeight="1">
+    <row r="35" spans="1:139" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="64"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="11" t="s">
         <v>117</v>
       </c>
@@ -3791,18 +3791,18 @@
         <v>25</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J35" s="41"/>
     </row>
-    <row r="36" spans="1:139" s="1" customFormat="1" ht="201" customHeight="1">
+    <row r="36" spans="1:139" s="1" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="62"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="11" t="s">
         <v>117</v>
       </c>
@@ -3821,14 +3821,14 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:139" s="1" customFormat="1" ht="373" customHeight="1">
+    <row r="37" spans="1:139" s="1" customFormat="1" ht="372.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="61" t="s">
+      <c r="B37" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="62"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="11" t="s">
         <v>117</v>
       </c>
@@ -3843,18 +3843,18 @@
         <v>14</v>
       </c>
       <c r="I37" s="40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J37" s="41"/>
     </row>
-    <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="61" t="s">
+      <c r="B38" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="62"/>
+      <c r="C38" s="56"/>
       <c r="D38" s="11" t="s">
         <v>117</v>
       </c>
@@ -3871,14 +3871,14 @@
       </c>
       <c r="J38" s="41"/>
     </row>
-    <row r="39" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="39" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="62"/>
+      <c r="C39" s="56"/>
       <c r="D39" s="11" t="s">
         <v>117</v>
       </c>
@@ -3893,14 +3893,14 @@
       <c r="I39" s="40"/>
       <c r="J39" s="41"/>
     </row>
-    <row r="40" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="40" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="64"/>
+      <c r="C40" s="66"/>
       <c r="D40" s="11" t="s">
         <v>117</v>
       </c>
@@ -3917,18 +3917,18 @@
         <v>30</v>
       </c>
       <c r="I40" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J40" s="41"/>
     </row>
-    <row r="41" spans="1:139" s="5" customFormat="1" ht="113" customHeight="1">
+    <row r="41" spans="1:139" s="5" customFormat="1" ht="113.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="62"/>
+      <c r="C41" s="56"/>
       <c r="D41" s="11" t="s">
         <v>117</v>
       </c>
@@ -3943,16 +3943,16 @@
         <v>5</v>
       </c>
       <c r="I41" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J41" s="41"/>
     </row>
-    <row r="42" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1">
+    <row r="42" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="66"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="60"/>
       <c r="D42" s="16"/>
       <c r="E42" s="18"/>
       <c r="F42" s="30"/>
@@ -4090,14 +4090,14 @@
       <c r="EH42" s="9"/>
       <c r="EI42" s="9"/>
     </row>
-    <row r="43" spans="1:139" s="5" customFormat="1" ht="177" customHeight="1">
+    <row r="43" spans="1:139" s="5" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="61" t="s">
+      <c r="B43" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="62"/>
+      <c r="C43" s="56"/>
       <c r="D43" s="13" t="s">
         <v>117</v>
       </c>
@@ -4118,14 +4118,14 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="44" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="64"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="13" t="s">
         <v>117</v>
       </c>
@@ -4140,18 +4140,18 @@
         <v>30</v>
       </c>
       <c r="I44" s="40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J44" s="41"/>
     </row>
-    <row r="45" spans="1:139" s="5" customFormat="1" ht="188" customHeight="1">
+    <row r="45" spans="1:139" s="5" customFormat="1" ht="188.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="62"/>
+      <c r="C45" s="56"/>
       <c r="D45" s="13" t="s">
         <v>117</v>
       </c>
@@ -4166,18 +4166,18 @@
         <v>12</v>
       </c>
       <c r="I45" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J45" s="41"/>
     </row>
-    <row r="46" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="46" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="62"/>
+      <c r="C46" s="56"/>
       <c r="D46" s="13" t="s">
         <v>144</v>
       </c>
@@ -4198,14 +4198,14 @@
       </c>
       <c r="J46" s="41"/>
     </row>
-    <row r="47" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="47" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" s="55" t="s">
         <v>197</v>
       </c>
-      <c r="B47" s="61" t="s">
-        <v>198</v>
-      </c>
-      <c r="C47" s="62"/>
+      <c r="C47" s="56"/>
       <c r="D47" s="13" t="s">
         <v>144</v>
       </c>
@@ -4220,14 +4220,14 @@
       <c r="I47" s="40"/>
       <c r="J47" s="41"/>
     </row>
-    <row r="48" spans="1:139" s="5" customFormat="1" ht="212" customHeight="1">
+    <row r="48" spans="1:139" s="5" customFormat="1" ht="212.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="64"/>
+      <c r="C48" s="66"/>
       <c r="D48" s="13" t="s">
         <v>88</v>
       </c>
@@ -4246,12 +4246,12 @@
       </c>
       <c r="J48" s="41"/>
     </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="49" spans="1:10" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15"/>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="62"/>
+      <c r="C49" s="56"/>
       <c r="D49" s="13" t="s">
         <v>4</v>
       </c>
@@ -4264,14 +4264,46 @@
       <c r="I49" s="36"/>
       <c r="J49" s="41"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="J50" s="41"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="J51" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B3:C3"/>
@@ -4288,38 +4320,6 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4340,7 +4340,7 @@
       <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4359,7 +4359,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change the file named xxh注意事项讲述
</commit_message>
<xml_diff>
--- a/Admin/2015-TH-XLP-流程及计分规则.xlsx
+++ b/Admin/2015-TH-XLP-流程及计分规则.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="0" windowWidth="24820" windowHeight="13460"/>
+    <workbookView xWindow="1305" yWindow="0" windowWidth="24825" windowHeight="13455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2593,16 +2593,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2611,12 +2626,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2627,26 +2636,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2941,31 +2944,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EI51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H47" sqref="H47"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="23" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.875" style="31" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="35" customWidth="1"/>
     <col min="8" max="8" width="19" style="35" customWidth="1"/>
-    <col min="9" max="9" width="58.6640625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="49.6640625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="3" customWidth="1"/>
-    <col min="12" max="13" width="16.33203125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="3"/>
+    <col min="9" max="9" width="58.625" style="36" customWidth="1"/>
+    <col min="10" max="10" width="49.625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="12.875" style="3" customWidth="1"/>
+    <col min="12" max="13" width="16.375" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1">
+    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="24.75" customHeight="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3015,14 +3018,14 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="114" customHeight="1">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
@@ -3041,14 +3044,14 @@
       <c r="I3" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="64" t="s">
         <v>183</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="68" customHeight="1">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>137</v>
       </c>
@@ -3062,16 +3065,16 @@
       <c r="G4" s="38"/>
       <c r="H4" s="39"/>
       <c r="I4" s="40"/>
-      <c r="J4" s="71"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="51" customHeight="1">
+      <c r="J4" s="65"/>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="11" t="s">
         <v>111</v>
       </c>
@@ -3084,16 +3087,16 @@
       </c>
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
-      <c r="J5" s="71"/>
-    </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" ht="52" customHeight="1">
+      <c r="J5" s="65"/>
+    </row>
+    <row r="6" spans="1:12" s="5" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="61"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="11" t="s">
         <v>111</v>
       </c>
@@ -3108,16 +3111,16 @@
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="40"/>
-      <c r="J6" s="72"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="99" customHeight="1">
+      <c r="J6" s="66"/>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="72" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -3136,14 +3139,14 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="188" customHeight="1">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="188.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="61"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="11" t="s">
         <v>111</v>
       </c>
@@ -3162,14 +3165,14 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" ht="48" customHeight="1">
+    <row r="9" spans="1:12" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="61"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="11" t="s">
         <v>111</v>
       </c>
@@ -3188,14 +3191,14 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="64.5" customHeight="1">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="11" t="s">
         <v>111</v>
       </c>
@@ -3215,14 +3218,14 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1">
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="11" t="s">
         <v>111</v>
       </c>
@@ -3239,14 +3242,14 @@
       <c r="I11" s="40"/>
       <c r="J11" s="44"/>
     </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" ht="117" customHeight="1">
+    <row r="12" spans="1:12" s="5" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="59"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="11" t="s">
         <v>102</v>
       </c>
@@ -3267,14 +3270,14 @@
       </c>
       <c r="J12" s="44"/>
     </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" ht="183" customHeight="1">
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="C13" s="59"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="11" t="s">
         <v>111</v>
       </c>
@@ -3295,14 +3298,14 @@
       </c>
       <c r="J13" s="46"/>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="81" customHeight="1">
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="59"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="11" t="s">
         <v>111</v>
       </c>
@@ -3323,14 +3326,14 @@
       </c>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="52" customHeight="1">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="61"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="11" t="s">
         <v>111</v>
       </c>
@@ -3345,14 +3348,14 @@
       <c r="I15" s="40"/>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="165" customHeight="1">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="59"/>
       <c r="D16" s="11" t="s">
         <v>111</v>
       </c>
@@ -3371,14 +3374,14 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="59"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="11" t="s">
         <v>111</v>
       </c>
@@ -3399,14 +3402,14 @@
       </c>
       <c r="J17" s="56"/>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="182" customHeight="1">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="182.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="59"/>
       <c r="D18" s="11" t="s">
         <v>111</v>
       </c>
@@ -3427,14 +3430,14 @@
       </c>
       <c r="J18" s="57"/>
     </row>
-    <row r="19" spans="1:10" s="5" customFormat="1" ht="98" customHeight="1">
+    <row r="19" spans="1:10" s="5" customFormat="1" ht="98.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="59"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="11" t="s">
         <v>111</v>
       </c>
@@ -3455,14 +3458,14 @@
       </c>
       <c r="J19" s="41"/>
     </row>
-    <row r="20" spans="1:10" s="5" customFormat="1" ht="203" customHeight="1">
+    <row r="20" spans="1:10" s="5" customFormat="1" ht="203.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="C20" s="59"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="11" t="s">
         <v>111</v>
       </c>
@@ -3485,12 +3488,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1">
+    <row r="21" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="63"/>
       <c r="D21" s="11"/>
       <c r="E21" s="17"/>
       <c r="F21" s="29"/>
@@ -3499,14 +3502,14 @@
       <c r="I21" s="40"/>
       <c r="J21" s="41"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="147" customHeight="1">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="67"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="11" t="s">
         <v>22</v>
       </c>
@@ -3527,14 +3530,14 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1">
+    <row r="23" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="11" t="s">
         <v>111</v>
       </c>
@@ -3555,14 +3558,14 @@
       </c>
       <c r="J23" s="41"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="121" customHeight="1">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="61"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="11" t="s">
         <v>111</v>
       </c>
@@ -3577,14 +3580,14 @@
       <c r="I24" s="40"/>
       <c r="J24" s="41"/>
     </row>
-    <row r="25" spans="1:10" s="5" customFormat="1" ht="268" customHeight="1">
+    <row r="25" spans="1:10" s="5" customFormat="1" ht="267.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="61"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="11" t="s">
         <v>111</v>
       </c>
@@ -3603,14 +3606,14 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="117" customHeight="1">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="59"/>
       <c r="D26" s="11" t="s">
         <v>111</v>
       </c>
@@ -3631,14 +3634,14 @@
       </c>
       <c r="J26" s="41"/>
     </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="121" customHeight="1">
+    <row r="27" spans="1:10" s="2" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="61"/>
+      <c r="C27" s="59"/>
       <c r="D27" s="11" t="s">
         <v>111</v>
       </c>
@@ -3655,14 +3658,14 @@
       </c>
       <c r="J27" s="41"/>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" ht="53" customHeight="1">
+    <row r="28" spans="1:10" s="2" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="58" t="s">
         <v>161</v>
       </c>
-      <c r="C28" s="61"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="11" t="s">
         <v>111</v>
       </c>
@@ -3677,14 +3680,14 @@
       <c r="I28" s="40"/>
       <c r="J28" s="41"/>
     </row>
-    <row r="29" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
+    <row r="29" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="59"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="11" t="s">
         <v>111</v>
       </c>
@@ -3705,14 +3708,14 @@
       </c>
       <c r="J29" s="41"/>
     </row>
-    <row r="30" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
+    <row r="30" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="C30" s="61"/>
+      <c r="C30" s="59"/>
       <c r="D30" s="11" t="s">
         <v>111</v>
       </c>
@@ -3729,14 +3732,14 @@
       </c>
       <c r="J30" s="41"/>
     </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
+    <row r="31" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="61"/>
+      <c r="C31" s="59"/>
       <c r="D31" s="11" t="s">
         <v>111</v>
       </c>
@@ -3755,14 +3758,14 @@
       </c>
       <c r="J31" s="41"/>
     </row>
-    <row r="32" spans="1:10" s="7" customFormat="1" ht="175" customHeight="1">
+    <row r="32" spans="1:10" s="7" customFormat="1" ht="174.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="59"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="11" t="s">
         <v>111</v>
       </c>
@@ -3783,12 +3786,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1">
+    <row r="33" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="65"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="63"/>
       <c r="D33" s="16"/>
       <c r="E33" s="18"/>
       <c r="F33" s="30"/>
@@ -3926,14 +3929,14 @@
       <c r="EH33" s="9"/>
       <c r="EI33" s="9"/>
     </row>
-    <row r="34" spans="1:139" s="2" customFormat="1" ht="117" customHeight="1">
+    <row r="34" spans="1:139" s="2" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="61"/>
+      <c r="C34" s="59"/>
       <c r="D34" s="11" t="s">
         <v>111</v>
       </c>
@@ -3952,14 +3955,14 @@
       </c>
       <c r="J34" s="41"/>
     </row>
-    <row r="35" spans="1:139" s="2" customFormat="1" ht="64.5" customHeight="1">
+    <row r="35" spans="1:139" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="59"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="11" t="s">
         <v>111</v>
       </c>
@@ -3980,14 +3983,14 @@
       </c>
       <c r="J35" s="41"/>
     </row>
-    <row r="36" spans="1:139" s="1" customFormat="1" ht="201" customHeight="1">
+    <row r="36" spans="1:139" s="1" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="61"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="11" t="s">
         <v>111</v>
       </c>
@@ -4006,14 +4009,14 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:139" s="1" customFormat="1" ht="373" customHeight="1">
+    <row r="37" spans="1:139" s="1" customFormat="1" ht="372.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="61"/>
+      <c r="C37" s="59"/>
       <c r="D37" s="11" t="s">
         <v>111</v>
       </c>
@@ -4032,14 +4035,14 @@
       </c>
       <c r="J37" s="41"/>
     </row>
-    <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B38" s="60" t="s">
+      <c r="B38" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="61"/>
+      <c r="C38" s="59"/>
       <c r="D38" s="11" t="s">
         <v>111</v>
       </c>
@@ -4056,14 +4059,14 @@
       </c>
       <c r="J38" s="41"/>
     </row>
-    <row r="39" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="39" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="B39" s="60" t="s">
+      <c r="B39" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="61"/>
+      <c r="C39" s="59"/>
       <c r="D39" s="11" t="s">
         <v>111</v>
       </c>
@@ -4078,14 +4081,14 @@
       <c r="I39" s="40"/>
       <c r="J39" s="41"/>
     </row>
-    <row r="40" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="40" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="59"/>
+      <c r="C40" s="61"/>
       <c r="D40" s="11" t="s">
         <v>111</v>
       </c>
@@ -4106,14 +4109,14 @@
       </c>
       <c r="J40" s="41"/>
     </row>
-    <row r="41" spans="1:139" s="5" customFormat="1" ht="113" customHeight="1">
+    <row r="41" spans="1:139" s="5" customFormat="1" ht="113.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="61"/>
+      <c r="C41" s="59"/>
       <c r="D41" s="11" t="s">
         <v>111</v>
       </c>
@@ -4132,12 +4135,12 @@
       </c>
       <c r="J41" s="41"/>
     </row>
-    <row r="42" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1">
+    <row r="42" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="64"/>
-      <c r="C42" s="65"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="63"/>
       <c r="D42" s="16"/>
       <c r="E42" s="18"/>
       <c r="F42" s="30"/>
@@ -4275,14 +4278,14 @@
       <c r="EH42" s="9"/>
       <c r="EI42" s="9"/>
     </row>
-    <row r="43" spans="1:139" s="5" customFormat="1" ht="177" customHeight="1">
+    <row r="43" spans="1:139" s="5" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="60" t="s">
+      <c r="B43" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="61"/>
+      <c r="C43" s="59"/>
       <c r="D43" s="13" t="s">
         <v>111</v>
       </c>
@@ -4303,14 +4306,14 @@
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="44" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="59"/>
+      <c r="C44" s="61"/>
       <c r="D44" s="13" t="s">
         <v>111</v>
       </c>
@@ -4329,14 +4332,14 @@
       </c>
       <c r="J44" s="41"/>
     </row>
-    <row r="45" spans="1:139" s="5" customFormat="1" ht="188" customHeight="1">
+    <row r="45" spans="1:139" s="5" customFormat="1" ht="188.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="61"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="13" t="s">
         <v>111</v>
       </c>
@@ -4355,14 +4358,14 @@
       </c>
       <c r="J45" s="41"/>
     </row>
-    <row r="46" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="46" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="61"/>
+      <c r="C46" s="59"/>
       <c r="D46" s="13" t="s">
         <v>130</v>
       </c>
@@ -4383,14 +4386,14 @@
       </c>
       <c r="J46" s="41"/>
     </row>
-    <row r="47" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="47" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B47" s="60" t="s">
+      <c r="B47" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="C47" s="61"/>
+      <c r="C47" s="59"/>
       <c r="D47" s="13" t="s">
         <v>130</v>
       </c>
@@ -4405,14 +4408,14 @@
       <c r="I47" s="40"/>
       <c r="J47" s="41"/>
     </row>
-    <row r="48" spans="1:139" s="5" customFormat="1" ht="212" customHeight="1">
+    <row r="48" spans="1:139" s="5" customFormat="1" ht="212.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="59"/>
+      <c r="C48" s="61"/>
       <c r="D48" s="13" t="s">
         <v>82</v>
       </c>
@@ -4431,12 +4434,12 @@
       </c>
       <c r="J48" s="41"/>
     </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" ht="102" customHeight="1">
+    <row r="49" spans="1:10" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15"/>
-      <c r="B49" s="60" t="s">
+      <c r="B49" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="61"/>
+      <c r="C49" s="59"/>
       <c r="D49" s="13" t="s">
         <v>4</v>
       </c>
@@ -4449,18 +4452,49 @@
       <c r="I49" s="36"/>
       <c r="J49" s="41"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="H50" s="35">
         <f>SUM(H1:H49)</f>
         <v>393</v>
       </c>
       <c r="J50" s="41"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="J51" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B49:C49"/>
@@ -4475,43 +4509,12 @@
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4528,7 +4531,7 @@
       <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4547,7 +4550,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed the file of scoring
</commit_message>
<xml_diff>
--- a/Admin/2015-TH-XLP-流程及计分规则.xlsx
+++ b/Admin/2015-TH-XLP-流程及计分规则.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="0" windowWidth="24825" windowHeight="13455"/>
+    <workbookView xWindow="1300" yWindow="0" windowWidth="24820" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="208">
   <si>
     <t>第1天</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -970,39 +970,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>每人填写调查问卷，截止时间21:30，延时者不得分（2分）
-每个人都撰写600字以上的日志到toyhouse，
-截止日期为21:30。延时者不得分（3分）                              展示文稿展以ppt格式，上交至teambition"清华大学2015
- XLP"项目中的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\展示\第五次展示\文件夹中                            命名为第x组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-截止日期为2015年1月28日7：00。延时上交者取消展示资格</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> 开场仪式是否迟到（2分）
  是否违反现场秩序（1分）
  服装是否得体（1分）
@@ -1010,6 +977,335 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>teambition任务发布（2分）
+项目经理在teambition “清华大学2015 XLP”项目的各自小组任务栏中发布任务，接受任务的成员在完成任务时通过teambition对任务反馈
+项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到22:00。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按时到达（2分）
+迟到者不得分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>每人填写调查问卷，截止时间21:30，延时者不得分（2分）
+每个人都撰写600字以上的日志到toyhouse，
+截止日期为21:30。延时者不得分（3分）                                             展示文稿展以ppt格式，上交至teambition"清华大学2015
+ XLP"项目中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的\展示\第三次展示\文件夹中                            命名为第x组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+截止日期为2015年1月27日7：00。延时上交者取消展示资格</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">每组必须有且仅有一个项目经理
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+团队组建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（2分） 
+上传第二次分组后的任务分工文档到teambition"清华大学2015 XLP"项目中的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\团队组建\第二次分组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹中，命名为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>第x组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">。截止日期2015年1月27日12:00  延时组不得分
+                                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上传注册信息和在Git上建立小组项目</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（2分）
+ 第二次分组后各组项目经理把组内成员的teambition账号，Git账号,（修改用户名为自己的姓名），小组项目地址，分组编号上传到teambition的“清华大学2015 XLP”项目的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\任务方账号\第二次分组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹内，命名为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>第x组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。上传文档为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Excel格式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">。截止日期2015年1月27日12:30，延时组不得分
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据顾老师的点评打分（15分）
+严格控制时间在要求时间之内(5分半），超时者不得分（3分）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据顾老师的点评打分（20分）
+严格控制时间在要求时间之内（6分钟），超时者不得分（3分）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有且仅有一个总项目经理                              原四组的子项目经理仍保留
+teambition任务发布
+2分
+子项目经理在teambition “清华大学2015 XLP”项目的各自小组任务栏中发布任务，接受任务的成员在完成任务时通过teambition对任务反馈
+子项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到22:00。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teambition任务发布
+2分
+ 项目经理在teambition “清华大学2015 XLP”项目的各自小组任务栏中发布任务，接受任务的成员在完成任务时通过teambition对任务反馈
+项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到15:00。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘉宾讲座(metatheory)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ray Doughty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t> Git技术团队依据团队现场游戏排名来计分，团队得分即为个人得分
+   第1名8分，第二名7分以此类推</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>货币市场交易记分（占总分的30%）分为两部分
+1.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>交易总金额</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（15%）：所有收税交易对应的金
+额总和为交易总金额
+交易总金额给分规则：以交易次数最多者为100%，该人得满分，交易次数在90%~100%之间的得90%，以此类推
+2.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>货币剩余量</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（15%）：最后活动结束时每个人手头的货币剩余量
+货币剩余量给分规则：以货币剩余量最多者为100%，该人得满分，交易次数在90%~100%之间的得90%，以此类推</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据顾老师的点评打分（25分）
+严格控制时间在要求时间之内（12分钟），超时者不得分（5分）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">            每组必须有且仅有一个项目经理        </t>
     </r>
@@ -1107,6 +1403,17 @@
 项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到22:00。
 </t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">会议记录要求叙述（下同）：
+1. 会议记录必须用md格式文件记录，同时配有少量图片视频等其他记录。此记录为本次会议的最重要的证据，让他人可以一目了然的了解会议的内容和意义。
+2. 我们将根据记录中的内容，给每人评分。
+3. 会议记录需要包括：
+① 记录中必须有明确的格式，如议题，内容，结论，最后分工等等。根据整体的结构清晰情况给分。【小组统一给分，总分为5分】
+② 有效思想及其提供者。【个人给分，有效思想越多，质量越高，给分越高，总分为10分】
+③ 最后需要有所有人的数字签名。【签名必须要个人签名，不得代签，被代签者扣5分。若缺少某同学签名，则该同学扣10分。】
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1116,7 +1423,7 @@
 可以使用3D打印制作出实物，记分组根据实物
 制作情况给分。（2分）
 若有实物制作，必须在当天17:00前完
-成若延时上交，其3分满分降为2分
+成若延时上交，其2分满分降为1分
 不制作实物不得分，也不扣分</t>
     </r>
     <r>
@@ -1138,8 +1445,7 @@
     <r>
       <t>讨论过程中必须使用罗伯特议事规则，635书面头
 脑风暴模版和商业模式画布三种工具其中的一到三种。（5分）
-各成员参与度、发言质量。（3分）                                 上传会议纪要到teambition"清华大学2015
- XLP"项目中的</t>
+各成员参与度、发言质量。（3分）                                 上传会议纪要到git各组各自项目</t>
     </r>
     <r>
       <rPr>
@@ -1151,7 +1457,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">会议记录\第一次分组\第一次会议                        </t>
+      <t xml:space="preserve">                                 </t>
     </r>
     <r>
       <rPr>
@@ -1174,7 +1480,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>第x组</t>
+      <t>第一次会议</t>
     </r>
     <r>
       <rPr>
@@ -1236,6 +1542,10 @@
       <t xml:space="preserve">
 截止日期为2015年1月26日13:10。延时上交者不得分                </t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>此次会议纪要中要明确</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1244,8 +1554,7 @@
 脑风暴模版和商业模式画布三种工具中一到三种。（5分）
 讨论过程中各成员参与度、发言质量。（3分）
  每个小组都必须持有会议展开的记录（文字，相片，视频等）
-并且上传至teambition"清华大学 2015XLP"
-的</t>
+上传会议纪要到git各组各自项目                                 命名为</t>
     </r>
     <r>
       <rPr>
@@ -1257,7 +1566,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">\会议记录\第一次分组\第二次会议 </t>
+      <t>第二次会议</t>
     </r>
     <r>
       <rPr>
@@ -1268,30 +1577,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>命名为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">第x组     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">             截至日期为18：30（20分)                                                                                   展示文稿展以ppt格式，上交至teambition"清华大学2015
+      <t xml:space="preserve">   截至日期为18：30（20分)                                                                                   展示文稿展以ppt格式，上交至teambition"清华大学2015
  XLP"项目中</t>
     </r>
     <r>
@@ -1345,249 +1631,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>teambition任务发布（2分）
-项目经理在teambition “清华大学2015 XLP”项目的各自小组任务栏中发布任务，接受任务的成员在完成任务时通过teambition对任务反馈
-项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到22:00。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>按时到达（2分）
-迟到者不得分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>之后的工作将在git上展开
-Git使用情况（占总分的40%）
-                                                                                                        上传注册信息和在Git上建立小组项目（2分）
- 第一次分组后各组项目经理把组内成员的teambition账号，Git账号,（修改用户名为自己的姓名），小组项目地址，分组编号上传到teambition的“清华大学2015 XLP”项目的\任务方账号\第一次分组文件夹内，命名为第x组。上传文档为Excel格式。截止日期2015年1月26日17:30 延时组全组成员不得分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>每人填写调查问卷，截止时间21:30，延时者不得分（2分）
-每个人都撰写600字以上的日志到toyhouse，
-截止日期为21:30。延时者不得分（3分）                                             展示文稿展以ppt格式，上交至teambition"清华大学2015
- XLP"项目中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的\展示\第三次展示\文件夹中                            命名为第x组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-截止日期为2015年1月27日7：00。延时上交者取消展示资格</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">每组必须有且仅有一个项目经理
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-团队组建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（2分） 
-上传第二次分组后的任务分工文档到teambition"清华大学2015 XLP"项目中的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\团队组建\第二次分组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹中，命名为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>第x组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">。截止日期2015年1月27日12:00  延时组不得分
-                                                    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>上传注册信息和在Git上建立小组项目</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（2分）
- 第二次分组后各组项目经理把组内成员的teambition账号，Git账号,（修改用户名为自己的姓名），小组项目地址，分组编号上传到teambition的“清华大学2015 XLP”项目的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\任务方账号\第二次分组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹内，命名为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>第x组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>。上传文档为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Excel格式</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">。截止日期2015年1月27日12:30，延时组不得分
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">讨论过程中必须使用罗伯特议事规则，635书面头
+    <r>
+      <t>讨论过程中必须使用罗伯特议事规则，635书面头
 脑风暴模版和商业模式画布三种工具中一到三种。。（5分）
 讨论过程中各成员参与度、发言质量。（3分）
 每个小组都必须持有会议展开的记录（文字，相片，视频）
-等并且上传至teambition"清华大学 2015XLP"的
-</t>
+等并且上传至git各小组项目中</t>
     </r>
     <r>
       <rPr>
@@ -1599,7 +1648,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">\会议记录\第二次分组\第三次会议 </t>
+      <t xml:space="preserve">    命名为第三次会议                        </t>
     </r>
     <r>
       <rPr>
@@ -1610,7 +1659,16 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 命名为</t>
+      <t>截至时间为11：00（20分）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>每人填写调查问卷，截止时间21:30，延时者不得分（2分）
+每个人都撰写600字以上的日志到toyhouse，
+截止日期为21:30。延时者不得分（3分）                              展示文稿展以ppt格式，上交至teambition"清华大学2015
+ XLP"项目中的</t>
     </r>
     <r>
       <rPr>
@@ -1622,7 +1680,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">第x组                    </t>
+      <t>\展示\第五次展示\文件夹中                            命名为第x组</t>
     </r>
     <r>
       <rPr>
@@ -1633,13 +1691,124 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>截至时间为11：00（20分）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据顾老师的点评打分（15分）
-严格控制时间在要求时间之内(5分半），超时者不得分（3分）</t>
+      <t xml:space="preserve">
+截止日期为2015年1月28日7：00。延时上交者取消展示资格</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文档要求：必须至少分工四组                                      （即原组成员不变，但可以通过交易形成暂时的雇佣关系，被雇佣者仍隶属与原组，但需在任务分工文档中注明）                                                          各组专做宪章、微电影、网页、实物其中之一
+关于筹备组工作，                                              由项目经理决定其是否专干（不再参与原组的工作），
+若专干，则也需要在文档中说明和备注筹备组与全组成员之间的协议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>所有成员必须统一参与一次整组讨论，进行分工
+讨论过程中必须使用罗伯特议事规则，635书面头
+脑风暴模版和商业模式画布三种工具中一到三种。（5分）
+讨论过程中各成员参与度、发言质量。（3分）
+必须持有会议展开的记录（文字，相片，视频等）
+并且上传会议纪要到git各组各自项目                                 命名为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>第五次会议</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  （20分）
+项目经理上传任务分工文档到teambition"清华大学2015 XLP"项
+目中的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\团队组建\任务方合组\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹中 命名为</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>任务方合组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。（2分）
+截止日期2015年1月28日12:00  延时全组不得分                                                              
+展示文稿展以ppt格式，上交至teambition"清华大学2015
+ XLP"项目中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的\展示\第六次展示\文件夹中                            命名为任务方合组</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+截止时间为13：10。延时上交者取消展示资格</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1648,8 +1817,7 @@
 脑风暴模版和商业模式画布三种工具中一到三种。（5分）
 讨论过程中各成员参与度、发言质量。（3分）
 每个小组都必须持有会议展开的记录（文字，相片，视频等）
-并且上传至teambition"清华大学 2015XLP"的
-\</t>
+并且上传上传会议纪要到git各组各自项目                                 命名为</t>
     </r>
     <r>
       <rPr>
@@ -1661,7 +1829,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>会议记录\第二次分组\第四次会议</t>
+      <t>第四次会议</t>
     </r>
     <r>
       <rPr>
@@ -1672,202 +1840,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  命名为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>第x组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                             截至日期为18：00（20分）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据顾老师的点评打分（20分）
-严格控制时间在要求时间之内（6分钟），超时者不得分（3分）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有且仅有一个总项目经理                              原四组的子项目经理仍保留
-teambition任务发布
-2分
-子项目经理在teambition “清华大学2015 XLP”项目的各自小组任务栏中发布任务，接受任务的成员在完成任务时通过teambition对任务反馈
-子项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到22:00。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">所有成员必须统一参与一次整组讨论，进行分工
-讨论过程中必须使用罗伯特议事规则，635书面头
-脑风暴模版和商业模式画布三种工具中一到三种。（5分）
-讨论过程中各成员参与度、发言质量。（3分）
-必须持有会议展开的记录（文字，相片，视频等）
-并且上传至teambition"清华大学 2015XLP"的
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">\会议记录\任务方合组\第五次会议 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 命名为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任务方合组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（20分）
-项目经理上传任务分工文档到teambition"清华大学2015 XLP"项
-目中的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\团队组建\任务方合组\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹中 命名为</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任务方合组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">。（2分）
-                                                              </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文档要求：必须至少分工四组                                      （即原组成员不变，但可以通过交易形成暂时的雇佣关系，被雇佣者仍隶属与原组，但需在任务分工文档中注明）                                                          各组专做宪章、微电影、网页、实物其中之一
-关于筹备组工作，                                              由项目经理决定其是否专干（不再参与原组的工作），
-若专干，则也需要在文档中说明和备注筹备组与全组成员之间的协议</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-截止日期2015年1月28日12:00  延时全组不得分
-展示文稿展以ppt格式，上交至teambition"清华大学2015
- XLP"项目中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的\展示\第六次展示\文件夹中                            命名为任务方合组</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-截止时间为13：10。延时上交者取消展示资格</t>
+      <t xml:space="preserve">                                              截至日期为18：00（20分）</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1878,8 +1851,7 @@
 脑风暴模版和商业模式画布三种工具中一到三种。（5分）
 讨论过程中各成员参与度、发言质量。（3分）
 必须持有会议展开的记录（文字，相片，视频等）
-并且上传至teambition"清华大学 2015XLP"的
-\</t>
+并且上传上传会议纪要到git各组各自项目                                 命名为</t>
     </r>
     <r>
       <rPr>
@@ -1891,7 +1863,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">会议记录\任务方合组\第六次会议 命名为任务方合组              </t>
+      <t xml:space="preserve">第六次会议 </t>
     </r>
     <r>
       <rPr>
@@ -1902,7 +1874,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>截止时期至12：00（20分）                                        展示文稿展以ppt格式，上交至teambition"清华大学2015
+      <t>（20分）                                             展示文稿展以ppt格式，上交至teambition"清华大学2015
  XLP"项目中的</t>
     </r>
     <r>
@@ -1944,85 +1916,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>teambition任务发布
-2分
- 项目经理在teambition “清华大学2015 XLP”项目的各自小组任务栏中发布任务，接受任务的成员在完成任务时通过teambition对任务反馈
-项目经理必须通过teambition给每个人发布命令，少一人少得1分，每天最少1条，组员对给自己的任务进行反馈，有几条任务没有反馈，就少得几分，直至当天本项得分为零为止。截止到15:00。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>嘉宾讲座(metatheory)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ray Doughty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t> Git技术团队依据团队现场游戏排名来计分，团队得分即为个人得分
-   第1名8分，第二名7分以此类推</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>货币市场交易记分（占总分的30%）分为两部分
-1.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>交易总金额</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（15%）：所有收税交易对应的金
-额总和为交易总金额
-交易总金额给分规则：以交易次数最多者为100%，该人得满分，交易次数在90%~100%之间的得90%，以此类推
-2.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>货币剩余量</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（15%）：最后活动结束时每个人手头的货币剩余量
-货币剩余量给分规则：以货币剩余量最多者为100%，该人得满分，交易次数在90%~100%之间的得90%，以此类推</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据顾老师的点评打分（25分）
-严格控制时间在要求时间之内（12分钟），超时者不得分（5分）</t>
+    <t>之后的工作将在git上展开
+Git使用情况（占总分的40%）
+每人的Git总分为510分。
+1. 其中记分组将保留300分，分别在八组进四组，四组进一组和最后发布会成品的三个时间节点给分，三次各占100分。
+此分数的给分细则如下：
+① 由记分组成员根据各组git项目中的成果状况，如宪章的质量，微电影的质量等因素，给出客观分数。【小组给分，总分50分】
+② 根据git 各组项目中的各时间节点的成果中数据的源作者贡献，两方面给分。【个人给分，总分50分】
+2. 剩余210分，在day1~3晚分发，每次分发70分。分数分发方式如下——对每一小组，分发总分为“总人数”乘以“70”。小组中的每个人进行不记名给分，给分对象为小组中包括自己在内的所有人。要求每人给分总分和小组分发总分相同。给分依据为各成员当天的git使用情况，频率，贡献等，其中最主要的依据为成员的git有效量，并且在每人上交的评分中需要给出对各成员（包括自己）评分的理由。
+给分必须公平公正，若被发现存在串通情况，记分组将毫不留情地扣除当天的git分数。
+【对git有效量作出简单的举例：如在宪章合并时，合并后采用的数据的源作者拥有较大的有效量；或者是在构建微电影时引用的视频的作者拥有较大的有效量。】
+所有同学都在当天晚上十点前把对小组成员的打分情况通过邮件上交到记分组（末尾注明组号和真实姓名），延时上交同学不得到当天的70分。邮箱为oceanneo@163.com
+记分组会在第二天早上分组前公布md格式的各组此部分给分情况。同学若没有异议，则在最后数字签名。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2640,16 +2545,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2944,31 +2846,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EI51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="H46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="23" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.875" style="31" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="31" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="35" customWidth="1"/>
     <col min="8" max="8" width="19" style="35" customWidth="1"/>
-    <col min="9" max="9" width="58.625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="49.625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="12.875" style="3" customWidth="1"/>
-    <col min="12" max="13" width="16.375" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.875" style="3"/>
+    <col min="9" max="9" width="58.6640625" style="36" customWidth="1"/>
+    <col min="10" max="10" width="49.6640625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="3" customWidth="1"/>
+    <col min="12" max="13" width="16.33203125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="14" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -3004,7 +2906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="24.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3018,7 +2920,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="114" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
@@ -3042,16 +2944,16 @@
         <v>4</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J3" s="64" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="68" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>137</v>
       </c>
@@ -3067,7 +2969,7 @@
       <c r="I4" s="40"/>
       <c r="J4" s="65"/>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="51" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>27</v>
       </c>
@@ -3089,7 +2991,7 @@
       <c r="I5" s="40"/>
       <c r="J5" s="65"/>
     </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" s="5" customFormat="1" ht="52" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>141</v>
       </c>
@@ -3113,7 +3015,7 @@
       <c r="I6" s="40"/>
       <c r="J6" s="66"/>
     </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="99" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>142</v>
       </c>
@@ -3139,7 +3041,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="188.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="188" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>47</v>
       </c>
@@ -3162,10 +3064,10 @@
       <c r="H8" s="39"/>
       <c r="I8" s="40"/>
       <c r="J8" s="42" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="5" customFormat="1" ht="48" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>144</v>
       </c>
@@ -3191,7 +3093,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" s="1" customFormat="1" ht="64.5" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>145</v>
       </c>
@@ -3218,7 +3120,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="64.5" customHeight="1">
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
@@ -3242,7 +3144,7 @@
       <c r="I11" s="40"/>
       <c r="J11" s="44"/>
     </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="5" customFormat="1" ht="117" customHeight="1">
       <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
@@ -3266,11 +3168,11 @@
         <v>5</v>
       </c>
       <c r="I12" s="45" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="J12" s="44"/>
     </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="218" customHeight="1">
       <c r="A13" s="15" t="s">
         <v>93</v>
       </c>
@@ -3294,11 +3196,13 @@
         <v>28</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="J13" s="46"/>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+      <c r="J13" s="46" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" ht="59" customHeight="1">
       <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
@@ -3326,19 +3230,19 @@
       </c>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" s="1" customFormat="1" ht="31" customHeight="1">
       <c r="A15" s="15" t="s">
         <v>148</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="11" t="s">
         <v>111</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="38" t="s">
@@ -3348,7 +3252,7 @@
       <c r="I15" s="40"/>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" s="1" customFormat="1" ht="409" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>149</v>
       </c>
@@ -3371,10 +3275,10 @@
       <c r="H16" s="39"/>
       <c r="I16" s="40"/>
       <c r="J16" s="55" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>150</v>
       </c>
@@ -3398,11 +3302,11 @@
         <v>8</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="J17" s="56"/>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="182.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="182" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>151</v>
       </c>
@@ -3426,11 +3330,11 @@
         <v>28</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="J18" s="57"/>
     </row>
-    <row r="19" spans="1:10" s="5" customFormat="1" ht="98.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" s="5" customFormat="1" ht="98" customHeight="1">
       <c r="A19" s="32" t="s">
         <v>37</v>
       </c>
@@ -3458,7 +3362,7 @@
       </c>
       <c r="J19" s="41"/>
     </row>
-    <row r="20" spans="1:10" s="5" customFormat="1" ht="203.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" s="5" customFormat="1" ht="203" customHeight="1">
       <c r="A20" s="33" t="s">
         <v>135</v>
       </c>
@@ -3482,13 +3386,13 @@
         <v>5</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="J20" s="41" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -3502,7 +3406,7 @@
       <c r="I21" s="40"/>
       <c r="J21" s="41"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="147" customHeight="1">
       <c r="A22" s="15" t="s">
         <v>40</v>
       </c>
@@ -3524,13 +3428,13 @@
         <v>2</v>
       </c>
       <c r="I22" s="40" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="J22" s="41" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.15">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="5" customFormat="1" ht="78" customHeight="1">
       <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
@@ -3558,7 +3462,7 @@
       </c>
       <c r="J23" s="41"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="121" customHeight="1">
       <c r="A24" s="15" t="s">
         <v>156</v>
       </c>
@@ -3580,7 +3484,7 @@
       <c r="I24" s="40"/>
       <c r="J24" s="41"/>
     </row>
-    <row r="25" spans="1:10" s="5" customFormat="1" ht="267.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" s="5" customFormat="1" ht="268" customHeight="1">
       <c r="A25" s="15" t="s">
         <v>104</v>
       </c>
@@ -3603,10 +3507,10 @@
       <c r="H25" s="39"/>
       <c r="I25" s="40"/>
       <c r="J25" s="47" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="117" customHeight="1">
       <c r="A26" s="15" t="s">
         <v>158</v>
       </c>
@@ -3630,11 +3534,13 @@
         <v>13</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="J26" s="41"/>
-    </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+      <c r="J26" s="41" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="2" customFormat="1" ht="121" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>159</v>
       </c>
@@ -3658,7 +3564,7 @@
       </c>
       <c r="J27" s="41"/>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" s="2" customFormat="1" ht="53" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>177</v>
       </c>
@@ -3680,7 +3586,7 @@
       <c r="I28" s="40"/>
       <c r="J28" s="41"/>
     </row>
-    <row r="29" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>178</v>
       </c>
@@ -3704,11 +3610,11 @@
         <v>18</v>
       </c>
       <c r="I29" s="40" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J29" s="41"/>
     </row>
-    <row r="30" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
       <c r="A30" s="10" t="s">
         <v>164</v>
       </c>
@@ -3732,7 +3638,7 @@
       </c>
       <c r="J30" s="41"/>
     </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" s="7" customFormat="1" ht="116.25" customHeight="1">
       <c r="A31" s="34" t="s">
         <v>105</v>
       </c>
@@ -3754,11 +3660,11 @@
         <v>28</v>
       </c>
       <c r="I31" s="40" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="J31" s="41"/>
     </row>
-    <row r="32" spans="1:10" s="7" customFormat="1" ht="174.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" s="7" customFormat="1" ht="175" customHeight="1">
       <c r="A32" s="10" t="s">
         <v>55</v>
       </c>
@@ -3780,13 +3686,13 @@
         <v>5</v>
       </c>
       <c r="I32" s="40" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="J32" s="41" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>15</v>
       </c>
@@ -3929,7 +3835,7 @@
       <c r="EH33" s="9"/>
       <c r="EI33" s="9"/>
     </row>
-    <row r="34" spans="1:139" s="2" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:139" s="2" customFormat="1" ht="117" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>40</v>
       </c>
@@ -3955,7 +3861,7 @@
       </c>
       <c r="J34" s="41"/>
     </row>
-    <row r="35" spans="1:139" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:139" s="2" customFormat="1" ht="64.5" customHeight="1">
       <c r="A35" s="10" t="s">
         <v>59</v>
       </c>
@@ -3979,11 +3885,11 @@
         <v>23</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="J35" s="41"/>
     </row>
-    <row r="36" spans="1:139" s="1" customFormat="1" ht="201" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:139" s="1" customFormat="1" ht="201" customHeight="1">
       <c r="A36" s="15" t="s">
         <v>62</v>
       </c>
@@ -4006,10 +3912,10 @@
       <c r="H36" s="39"/>
       <c r="I36" s="40"/>
       <c r="J36" s="41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:139" s="1" customFormat="1" ht="372.95" customHeight="1" x14ac:dyDescent="0.15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:139" s="1" customFormat="1" ht="373" customHeight="1">
       <c r="A37" s="15" t="s">
         <v>63</v>
       </c>
@@ -4031,11 +3937,13 @@
         <v>30</v>
       </c>
       <c r="I37" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="J37" s="41"/>
-    </row>
-    <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+      <c r="J37" s="41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A38" s="15" t="s">
         <v>177</v>
       </c>
@@ -4059,7 +3967,7 @@
       </c>
       <c r="J38" s="41"/>
     </row>
-    <row r="39" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A39" s="15" t="s">
         <v>179</v>
       </c>
@@ -4081,7 +3989,7 @@
       <c r="I39" s="40"/>
       <c r="J39" s="41"/>
     </row>
-    <row r="40" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A40" s="15" t="s">
         <v>68</v>
       </c>
@@ -4109,7 +4017,7 @@
       </c>
       <c r="J40" s="41"/>
     </row>
-    <row r="41" spans="1:139" s="5" customFormat="1" ht="113.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:139" s="5" customFormat="1" ht="113" customHeight="1">
       <c r="A41" s="15" t="s">
         <v>69</v>
       </c>
@@ -4135,7 +4043,7 @@
       </c>
       <c r="J41" s="41"/>
     </row>
-    <row r="42" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:139" s="8" customFormat="1" ht="33" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>71</v>
       </c>
@@ -4278,7 +4186,7 @@
       <c r="EH42" s="9"/>
       <c r="EI42" s="9"/>
     </row>
-    <row r="43" spans="1:139" s="5" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:139" s="5" customFormat="1" ht="177" customHeight="1">
       <c r="A43" s="15" t="s">
         <v>72</v>
       </c>
@@ -4303,10 +4211,10 @@
         <v>126</v>
       </c>
       <c r="J43" s="41" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A44" s="15" t="s">
         <v>74</v>
       </c>
@@ -4328,11 +4236,11 @@
         <v>30</v>
       </c>
       <c r="I44" s="40" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="J44" s="41"/>
     </row>
-    <row r="45" spans="1:139" s="5" customFormat="1" ht="188.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:139" s="5" customFormat="1" ht="188" customHeight="1">
       <c r="A45" s="15" t="s">
         <v>176</v>
       </c>
@@ -4354,11 +4262,11 @@
         <v>28</v>
       </c>
       <c r="I45" s="40" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="J45" s="41"/>
     </row>
-    <row r="46" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A46" s="15" t="s">
         <v>77</v>
       </c>
@@ -4386,7 +4294,7 @@
       </c>
       <c r="J46" s="41"/>
     </row>
-    <row r="47" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A47" s="15" t="s">
         <v>166</v>
       </c>
@@ -4408,7 +4316,7 @@
       <c r="I47" s="40"/>
       <c r="J47" s="41"/>
     </row>
-    <row r="48" spans="1:139" s="5" customFormat="1" ht="212.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:139" s="5" customFormat="1" ht="212" customHeight="1">
       <c r="A48" s="15" t="s">
         <v>80</v>
       </c>
@@ -4434,7 +4342,7 @@
       </c>
       <c r="J48" s="41"/>
     </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:10" s="5" customFormat="1" ht="102" customHeight="1">
       <c r="A49" s="15"/>
       <c r="B49" s="58" t="s">
         <v>65</v>
@@ -4452,14 +4360,14 @@
       <c r="I49" s="36"/>
       <c r="J49" s="41"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:10">
       <c r="H50" s="35">
         <f>SUM(H1:H49)</f>
         <v>393</v>
       </c>
       <c r="J50" s="41"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:10">
       <c r="J51" s="41"/>
     </row>
   </sheetData>
@@ -4514,7 +4422,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4531,7 +4439,7 @@
       <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4550,7 +4458,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>